<commit_message>
Fixed list index issues that arose when values had to be removed due to negative log operations. May have to return for edge cases. See comments in Operation.extract_phase(...)
</commit_message>
<xml_diff>
--- a/Tests/1/Test_SingleRun5.xlsx
+++ b/Tests/1/Test_SingleRun5.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Vial #</t>
   </si>
@@ -143,7 +143,10 @@
     <t>End</t>
   </si>
   <si>
-    <t>Run4</t>
+    <t>Run5</t>
+  </si>
+  <si>
+    <t>Phase I Corrected</t>
   </si>
 </sst>
 </file>
@@ -277,7 +280,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -302,7 +305,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -323,30 +325,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -362,6 +352,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,7 +671,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,61 +682,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="29">
-        <v>1811.9839999999999</v>
+      <c r="B2" s="28"/>
+      <c r="C2" s="42">
+        <v>17875.075000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="30">
-        <v>5589.2</v>
+      <c r="B3" s="28"/>
+      <c r="C3" s="41">
+        <v>6513.4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="31">
-        <v>2353.1</v>
+      <c r="B4" s="28"/>
+      <c r="C4" s="40">
+        <v>1336.9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="32">
-        <v>0.53549000000000024</v>
+      <c r="B5" s="28"/>
+      <c r="C5" s="43">
+        <v>0.58800000000000008</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="33">
-        <v>1.0505677145283143</v>
+      <c r="B6" s="28"/>
+      <c r="C6" s="44">
+        <v>1.0394621801631903</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="28">
+      <c r="B7" s="28"/>
+      <c r="C7" s="25">
         <v>60</v>
       </c>
     </row>
@@ -753,240 +755,240 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="25">
-        <v>29940.6</v>
+      <c r="C9" s="35">
+        <v>39593.199999999997</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="25">
-        <v>8517.7999999999993</v>
+      <c r="C10" s="35">
+        <v>10341.4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="25">
-        <v>3472</v>
+      <c r="C11" s="35">
+        <v>4221.1000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>4</v>
       </c>
-      <c r="C12" s="25">
-        <v>1776.3</v>
+      <c r="C12" s="35">
+        <v>2157.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="25">
-        <v>359.7</v>
+      <c r="C13" s="35">
+        <v>1332.3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C14" s="25">
-        <v>1566.4</v>
+      <c r="C14" s="35">
+        <v>912.6</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="C15" s="25">
-        <v>857</v>
+      <c r="C15" s="35">
+        <v>618.79999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>8</v>
       </c>
-      <c r="C16" s="25">
-        <v>684.6</v>
+      <c r="C16" s="35">
+        <v>547.29999999999995</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>9</v>
       </c>
-      <c r="C17" s="25">
-        <v>486.7</v>
+      <c r="C17" s="35">
+        <v>490.6</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>10</v>
       </c>
-      <c r="C18" s="25">
-        <v>412</v>
+      <c r="C18" s="35">
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>11.5</v>
       </c>
-      <c r="C19" s="25">
-        <v>352</v>
+      <c r="C19" s="35">
+        <v>391.4</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>13</v>
       </c>
-      <c r="C20" s="25">
-        <v>341.5</v>
+      <c r="C20" s="35">
+        <v>250.9</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>14.5</v>
       </c>
-      <c r="C21" s="25">
-        <v>288.60000000000002</v>
+      <c r="C21" s="35">
+        <v>287.7</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>16</v>
       </c>
-      <c r="C22" s="25">
-        <v>241.2</v>
+      <c r="C22" s="35">
+        <v>269.2</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>17.5</v>
       </c>
-      <c r="C23" s="25">
-        <v>239.6</v>
+      <c r="C23" s="35">
+        <v>218.7</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>19</v>
       </c>
-      <c r="C24" s="25">
-        <v>207.2</v>
+      <c r="C24" s="35">
+        <v>190.8</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>20.5</v>
       </c>
-      <c r="C25" s="25">
-        <v>166.8</v>
+      <c r="C25" s="35">
+        <v>190.9</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>22</v>
       </c>
-      <c r="C26" s="25">
-        <v>196.9</v>
+      <c r="C26" s="35">
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>23.5</v>
       </c>
-      <c r="C27" s="25">
-        <v>154.4</v>
+      <c r="C27" s="35">
+        <v>129.9</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <v>25</v>
       </c>
-      <c r="C28" s="25">
-        <v>149.1</v>
+      <c r="C28" s="35">
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <v>27</v>
       </c>
-      <c r="C29" s="25">
-        <v>132.9</v>
+      <c r="C29" s="35">
+        <v>125.3</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>29</v>
       </c>
-      <c r="C30" s="25">
-        <v>173.1</v>
+      <c r="C30" s="35">
+        <v>132.1</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
         <v>31</v>
       </c>
-      <c r="C31" s="25">
-        <v>146.80000000000001</v>
+      <c r="C31" s="35">
+        <v>108.5</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
         <v>33</v>
       </c>
-      <c r="C32" s="25">
-        <v>164.2</v>
+      <c r="C32" s="35">
+        <v>134.30000000000001</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>35</v>
       </c>
-      <c r="C33" s="25">
-        <v>178.2</v>
+      <c r="C33" s="35">
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
         <v>37</v>
       </c>
-      <c r="C34" s="25">
-        <v>132.6</v>
+      <c r="C34" s="35">
+        <v>150.69999999999999</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <v>39</v>
       </c>
-      <c r="C35" s="25">
-        <v>146.5</v>
+      <c r="C35" s="35">
+        <v>125.2</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="3">
         <v>41</v>
       </c>
-      <c r="C36" s="25">
-        <v>131.9</v>
+      <c r="C36" s="35">
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="3">
         <v>43</v>
       </c>
-      <c r="C37" s="25">
-        <v>130.30000000000001</v>
+      <c r="C37" s="35">
+        <v>105.3</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="3">
         <v>45</v>
       </c>
-      <c r="C38" s="25">
-        <v>100.2</v>
+      <c r="C38" s="35">
+        <v>105.4</v>
       </c>
     </row>
   </sheetData>
@@ -1007,8 +1009,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A318" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F333" sqref="F333"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,17 +1021,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="41"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="36">
-        <v>1811.9839999999999</v>
+        <v>17875.075000000001</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -1044,12 +1046,12 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="37">
-        <v>5589.2</v>
+      <c r="B3" s="28"/>
+      <c r="C3" s="39">
+        <v>6513.4</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -1064,12 +1066,12 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="38">
-        <v>2353.1</v>
+      <c r="B4" s="28"/>
+      <c r="C4" s="40">
+        <v>1336.9</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -1084,12 +1086,12 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="39">
-        <v>0.53549000000000024</v>
+      <c r="B5" s="28"/>
+      <c r="C5" s="38">
+        <v>0.58800000000000008</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -1104,20 +1106,20 @@
       <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="40">
-        <v>1.0505677145283143</v>
+      <c r="B6" s="28"/>
+      <c r="C6" s="37">
+        <v>1.0394621801631903</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="35">
+      <c r="B7" s="28"/>
+      <c r="C7" s="27">
         <v>60</v>
       </c>
       <c r="D7" s="5"/>
@@ -1133,527 +1135,526 @@
       <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="23">
+      <c r="B8" s="31"/>
+      <c r="C8" s="22">
         <v>45</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="45"/>
+      <c r="B9" s="32"/>
       <c r="C9">
         <f>C16+C10</f>
-        <v>28.659506599261839</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
+        <v>3.88995527033891</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="43"/>
+      <c r="B10" s="30"/>
       <c r="C10">
         <f>60*(C13-(C22/C21)*EXP(-1*C21*C8))/C2/C7</f>
-        <v>6.8338450997208051</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
+        <v>0.69092818857175486</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="43"/>
+      <c r="B11" s="30"/>
       <c r="C11">
         <f>C16/C9</f>
-        <v>0.76155049717789569</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="17"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
+        <v>0.82238145671233953</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="16"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="43"/>
+      <c r="B12" s="30"/>
       <c r="C12">
         <f>C9*C17/(3*0.693)</f>
-        <v>237.78390406403778</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
+        <v>21.389810016036517</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="18">
+      <c r="B13" s="30"/>
+      <c r="C13" s="17">
         <f>(C3+C4)/C5</f>
-        <v>14831.836262115065</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
+        <v>13350.850340136052</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="18">
-        <f>C196</f>
-        <v>10</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
+      <c r="C14" s="17">
+        <v>6</v>
+      </c>
+      <c r="D14" s="17"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="17">
         <v>30</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
-      <c r="B16" s="21" t="s">
+      <c r="A16" s="29"/>
+      <c r="B16" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C16">
         <f>60*C22/(C$2*(1-EXP(-1*C21*60)))</f>
-        <v>21.825661499541035</v>
-      </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
+        <v>3.1990270817671553</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
-      <c r="B17" s="22" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="17">
         <f>0.693/C21</f>
-        <v>17.249171224806332</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
+        <v>11.431857677753076</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
-      <c r="B18" s="22" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C18">
-        <f>RSQ(C145:C164,B145:B164)</f>
-        <v>0.8676488819735938</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
+        <f>RSQ(C141:C164,B141:B164)</f>
+        <v>0.82697132814732521</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
-      <c r="B19" s="22" t="s">
+      <c r="A19" s="29"/>
+      <c r="B19" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="18">
-        <f>SLOPE(C145:C164,B145:B164)</f>
-        <v>-1.7445003599395947E-2</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
+      <c r="C19" s="17">
+        <f>SLOPE(C141:C164,B141:B164)</f>
+        <v>-2.6322218364293656E-2</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="42"/>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="29"/>
+      <c r="B20" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="18">
-        <f>INTERCEPT(C145:C164,B145:B164)</f>
-        <v>2.7781236457697607</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
+      <c r="C20" s="17">
+        <f>INTERCEPT(C141:C164,B141:B164)</f>
+        <v>2.9675281814410219</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="22" t="s">
+      <c r="A21" s="29"/>
+      <c r="B21" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="17">
         <f>ABS(C19)*2.303</f>
-        <v>4.0175843289408861E-2</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
+        <v>6.0620068892968289E-2</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="29"/>
+      <c r="B22" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="17">
         <f>10^C20</f>
-        <v>599.9618640285571</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
+        <v>927.95770350310067</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="17">
         <f>C291</f>
-        <v>5</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
+        <v>2</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
-      <c r="B24" s="21" t="s">
+      <c r="A24" s="29"/>
+      <c r="B24" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="17">
         <f>C196</f>
-        <v>10</v>
-      </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
+        <v>6</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
-      <c r="B25" s="21" t="s">
+      <c r="A25" s="29"/>
+      <c r="B25" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C25">
         <f>60*C31/(C$2*(1-EXP(-1*C30*60)))</f>
-        <v>1141.1036187048715</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
+        <v>144.49691303074499</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="22" t="s">
+      <c r="A26" s="29"/>
+      <c r="B26" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="17">
         <f>0.693/C30</f>
-        <v>1.5265676164854809</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
+        <v>1.0805887600827708</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="22" t="s">
+      <c r="A27" s="29"/>
+      <c r="B27" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C27">
-        <f>RSQ(C298:C302,B298:B302)</f>
-        <v>0.97171858170986258</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
+        <f>RSQ(C295:C298,B295:B298)</f>
+        <v>0.99349301294631553</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="22" t="s">
+      <c r="A28" s="29"/>
+      <c r="B28" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="18">
-        <f>SLOPE(C298:C302,B298:B302)</f>
-        <v>-0.19711662349821987</v>
-      </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
+      <c r="C28" s="17">
+        <f>SLOPE(C295:C298,B295:B298)</f>
+        <v>-0.27847027955417031</v>
+      </c>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
-      <c r="B29" s="22" t="s">
+      <c r="A29" s="29"/>
+      <c r="B29" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="18">
-        <f>INTERCEPT(C298:C302,B298:B302)</f>
-        <v>4.5373281907299532</v>
-      </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
+      <c r="C29" s="17">
+        <f>INTERCEPT(C295:C298,B295:B298)</f>
+        <v>4.6339551914133557</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="22" t="s">
+      <c r="A30" s="29"/>
+      <c r="B30" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="17">
         <f>ABS(C28)*2.303</f>
-        <v>0.45395958391640034</v>
-      </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
+        <v>0.64131705381325421</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="22" t="s">
+      <c r="A31" s="29"/>
+      <c r="B31" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="17">
         <f>10^C29</f>
-        <v>34461.02499053772</v>
-      </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
+        <v>43048.219294884067</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
-      <c r="B33" s="21" t="s">
+      <c r="A33" s="29"/>
+      <c r="B33" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="18">
+      <c r="C33" s="17">
         <f>C291</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -1668,34 +1669,34 @@
       <c r="N33" s="7"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
-      <c r="B34" s="21" t="s">
+      <c r="A34" s="29"/>
+      <c r="B34" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C34">
         <f>60*C40/(C$2*(1-EXP(-1*C39*60)))</f>
-        <v>19325.473306186552</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
+        <v>1312.0642842160021</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="42"/>
-      <c r="B35" s="22" t="s">
+      <c r="A35" s="29"/>
+      <c r="B35" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="17">
         <f>0.693/C39</f>
-        <v>0.2494042704725894</v>
+        <v>0.32527850066421321</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -1710,13 +1711,13 @@
       <c r="N35" s="7"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="22" t="s">
+      <c r="A36" s="29"/>
+      <c r="B36" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C36">
         <f>RSQ(C324:C327,B324:B327)</f>
-        <v>0.99999999999999956</v>
+        <v>1</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -1731,13 +1732,13 @@
       <c r="N36" s="7"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
-      <c r="B37" s="22" t="s">
+      <c r="A37" s="29"/>
+      <c r="B37" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="17">
         <f>SLOPE(C324:C327,B324:B327)</f>
-        <v>-1.2065224606345102</v>
+        <v>-0.92508989524019114</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -1752,13 +1753,13 @@
       <c r="N37" s="7"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
-      <c r="B38" s="22" t="s">
+      <c r="A38" s="29"/>
+      <c r="B38" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="18">
+      <c r="C38" s="17">
         <f>INTERCEPT(C324:C327,B324:B327)</f>
-        <v>5.7661332472724087</v>
+        <v>5.5920517359956552</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -1773,13 +1774,13 @@
       <c r="N38" s="7"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
-      <c r="B39" s="22" t="s">
+      <c r="A39" s="29"/>
+      <c r="B39" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="17">
         <f>ABS(C37)*2.303</f>
-        <v>2.7786212268412767</v>
+        <v>2.1304820287381601</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
@@ -1794,13 +1795,13 @@
       <c r="N39" s="7"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
-      <c r="B40" s="22" t="s">
+      <c r="A40" s="29"/>
+      <c r="B40" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="18">
+      <c r="C40" s="17">
         <f>10^C38</f>
-        <v>583624.1403872855</v>
+        <v>390887.45808637259</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
@@ -1840,8 +1841,8 @@
       <c r="B42" s="3">
         <v>1</v>
       </c>
-      <c r="C42" s="26">
-        <v>29940.6</v>
+      <c r="C42" s="34">
+        <v>39593.199999999997</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -1859,8 +1860,8 @@
       <c r="B43" s="3">
         <v>2</v>
       </c>
-      <c r="C43" s="26">
-        <v>8517.7999999999993</v>
+      <c r="C43" s="34">
+        <v>10341.4</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -1878,8 +1879,8 @@
       <c r="B44" s="3">
         <v>3</v>
       </c>
-      <c r="C44" s="26">
-        <v>3472</v>
+      <c r="C44" s="34">
+        <v>4221.1000000000004</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -1897,8 +1898,8 @@
       <c r="B45" s="4">
         <v>4</v>
       </c>
-      <c r="C45" s="26">
-        <v>1776.3</v>
+      <c r="C45" s="34">
+        <v>2157.5</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -1916,8 +1917,8 @@
       <c r="B46" s="3">
         <v>5</v>
       </c>
-      <c r="C46" s="26">
-        <v>359.7</v>
+      <c r="C46" s="34">
+        <v>1332.3</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -1935,8 +1936,8 @@
       <c r="B47" s="3">
         <v>6</v>
       </c>
-      <c r="C47" s="26">
-        <v>1566.4</v>
+      <c r="C47" s="34">
+        <v>912.6</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
@@ -1954,8 +1955,8 @@
       <c r="B48" s="3">
         <v>7</v>
       </c>
-      <c r="C48" s="26">
-        <v>857</v>
+      <c r="C48" s="34">
+        <v>618.79999999999995</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -1973,8 +1974,8 @@
       <c r="B49" s="3">
         <v>8</v>
       </c>
-      <c r="C49" s="26">
-        <v>684.6</v>
+      <c r="C49" s="34">
+        <v>547.29999999999995</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -1992,8 +1993,8 @@
       <c r="B50" s="3">
         <v>9</v>
       </c>
-      <c r="C50" s="26">
-        <v>486.7</v>
+      <c r="C50" s="34">
+        <v>490.6</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
@@ -2011,8 +2012,8 @@
       <c r="B51" s="4">
         <v>10</v>
       </c>
-      <c r="C51" s="26">
-        <v>412</v>
+      <c r="C51" s="34">
+        <v>344</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
@@ -2030,8 +2031,8 @@
       <c r="B52" s="4">
         <v>11.5</v>
       </c>
-      <c r="C52" s="26">
-        <v>352</v>
+      <c r="C52" s="34">
+        <v>391.4</v>
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
@@ -2049,8 +2050,8 @@
       <c r="B53" s="3">
         <v>13</v>
       </c>
-      <c r="C53" s="26">
-        <v>341.5</v>
+      <c r="C53" s="34">
+        <v>250.9</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
@@ -2067,8 +2068,8 @@
       <c r="B54" s="3">
         <v>14.5</v>
       </c>
-      <c r="C54" s="26">
-        <v>288.60000000000002</v>
+      <c r="C54" s="34">
+        <v>287.7</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
@@ -2086,8 +2087,8 @@
       <c r="B55" s="3">
         <v>16</v>
       </c>
-      <c r="C55" s="26">
-        <v>241.2</v>
+      <c r="C55" s="34">
+        <v>269.2</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -2105,8 +2106,8 @@
       <c r="B56" s="3">
         <v>17.5</v>
       </c>
-      <c r="C56" s="26">
-        <v>239.6</v>
+      <c r="C56" s="34">
+        <v>218.7</v>
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
@@ -2124,8 +2125,8 @@
       <c r="B57" s="3">
         <v>19</v>
       </c>
-      <c r="C57" s="26">
-        <v>207.2</v>
+      <c r="C57" s="34">
+        <v>190.8</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
@@ -2143,8 +2144,8 @@
       <c r="B58" s="3">
         <v>20.5</v>
       </c>
-      <c r="C58" s="26">
-        <v>166.8</v>
+      <c r="C58" s="34">
+        <v>190.9</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
@@ -2162,8 +2163,8 @@
       <c r="B59" s="3">
         <v>22</v>
       </c>
-      <c r="C59" s="26">
-        <v>196.9</v>
+      <c r="C59" s="34">
+        <v>176</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
@@ -2181,8 +2182,8 @@
       <c r="B60" s="3">
         <v>23.5</v>
       </c>
-      <c r="C60" s="26">
-        <v>154.4</v>
+      <c r="C60" s="34">
+        <v>129.9</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
@@ -2200,8 +2201,8 @@
       <c r="B61" s="3">
         <v>25</v>
       </c>
-      <c r="C61" s="26">
-        <v>149.1</v>
+      <c r="C61" s="34">
+        <v>130</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
@@ -2219,8 +2220,8 @@
       <c r="B62" s="3">
         <v>27</v>
       </c>
-      <c r="C62" s="26">
-        <v>132.9</v>
+      <c r="C62" s="34">
+        <v>125.3</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
@@ -2238,8 +2239,8 @@
       <c r="B63" s="3">
         <v>29</v>
       </c>
-      <c r="C63" s="26">
-        <v>173.1</v>
+      <c r="C63" s="34">
+        <v>132.1</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
@@ -2257,64 +2258,64 @@
       <c r="B64" s="3">
         <v>31</v>
       </c>
-      <c r="C64" s="26">
-        <v>146.80000000000001</v>
+      <c r="C64" s="34">
+        <v>108.5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" s="3">
         <v>33</v>
       </c>
-      <c r="C65" s="26">
-        <v>164.2</v>
+      <c r="C65" s="34">
+        <v>134.30000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" s="3">
         <v>35</v>
       </c>
-      <c r="C66" s="26">
-        <v>178.2</v>
+      <c r="C66" s="34">
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" s="3">
         <v>37</v>
       </c>
-      <c r="C67" s="26">
-        <v>132.6</v>
+      <c r="C67" s="34">
+        <v>150.69999999999999</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68" s="3">
         <v>39</v>
       </c>
-      <c r="C68" s="26">
-        <v>146.5</v>
+      <c r="C68" s="34">
+        <v>125.2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" s="3">
         <v>41</v>
       </c>
-      <c r="C69" s="26">
-        <v>131.9</v>
+      <c r="C69" s="34">
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" s="3">
         <v>43</v>
       </c>
-      <c r="C70" s="26">
-        <v>130.30000000000001</v>
+      <c r="C70" s="34">
+        <v>105.3</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71" s="3">
         <v>45</v>
       </c>
-      <c r="C71" s="26">
-        <v>100.2</v>
+      <c r="C71" s="34">
+        <v>105.4</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2329,270 +2330,270 @@
       <c r="B73" s="3">
         <v>1</v>
       </c>
-      <c r="C73" s="24">
+      <c r="C73" s="23">
         <f>C42*C$6</f>
-        <v>31454.627713606445</v>
+        <v>41155.633991637224</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B74" s="3">
         <v>2</v>
       </c>
-      <c r="C74" s="24">
+      <c r="C74" s="23">
         <f t="shared" ref="C74:C102" si="0">C43*C$6</f>
-        <v>8948.5256788092756</v>
+        <v>10749.494189939614</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" s="3">
         <v>3</v>
       </c>
-      <c r="C75" s="24">
+      <c r="C75" s="23">
         <f t="shared" si="0"/>
-        <v>3647.5711048423072</v>
+        <v>4387.6738086868427</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76" s="4">
         <v>4</v>
       </c>
-      <c r="C76" s="24">
+      <c r="C76" s="23">
         <f t="shared" si="0"/>
-        <v>1866.1234313166447</v>
+        <v>2242.6396537020828</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77" s="3">
         <v>5</v>
       </c>
-      <c r="C77" s="24">
+      <c r="C77" s="23">
         <f t="shared" si="0"/>
-        <v>377.88920691583468</v>
+        <v>1384.8754626314183</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78" s="3">
         <v>6</v>
       </c>
-      <c r="C78" s="24">
+      <c r="C78" s="23">
         <f t="shared" si="0"/>
-        <v>1645.6092680371517</v>
+        <v>948.61318561692747</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B79" s="3">
         <v>7</v>
       </c>
-      <c r="C79" s="24">
+      <c r="C79" s="23">
         <f t="shared" si="0"/>
-        <v>900.33653135076543</v>
+        <v>643.21919708498206</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80" s="3">
         <v>8</v>
       </c>
-      <c r="C80" s="24">
+      <c r="C80" s="23">
         <f t="shared" si="0"/>
-        <v>719.21865736608402</v>
+        <v>568.89765120331401</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="3">
         <v>9</v>
       </c>
-      <c r="C81" s="24">
+      <c r="C81" s="23">
         <f t="shared" si="0"/>
-        <v>511.31130666093054</v>
+        <v>509.96014558806115</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="4">
         <v>10</v>
       </c>
-      <c r="C82" s="24">
+      <c r="C82" s="23">
         <f t="shared" si="0"/>
-        <v>432.83389838566552</v>
+        <v>357.57498997613743</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="4">
         <v>11.5</v>
       </c>
-      <c r="C83" s="24">
+      <c r="C83" s="23">
         <f t="shared" si="0"/>
-        <v>369.79983551396663</v>
+        <v>406.84549731587265</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="3">
         <v>13</v>
       </c>
-      <c r="C84" s="24">
+      <c r="C84" s="23">
         <f t="shared" si="0"/>
-        <v>358.76887451141937</v>
+        <v>260.80106100294444</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="3">
         <v>14.5</v>
       </c>
-      <c r="C85" s="24">
+      <c r="C85" s="23">
         <f t="shared" si="0"/>
-        <v>303.19384241287156</v>
+        <v>299.05326923294984</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="3">
         <v>16</v>
       </c>
-      <c r="C86" s="24">
+      <c r="C86" s="23">
         <f t="shared" si="0"/>
-        <v>253.39693274422939</v>
+        <v>279.82321889993079</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="3">
         <v>17.5</v>
       </c>
-      <c r="C87" s="24">
+      <c r="C87" s="23">
         <f t="shared" si="0"/>
-        <v>251.71602440098411</v>
+        <v>227.3303788016897</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="3">
         <v>19</v>
       </c>
-      <c r="C88" s="24">
+      <c r="C88" s="23">
         <f t="shared" si="0"/>
-        <v>217.67763045026672</v>
+        <v>198.32938397513672</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="3">
         <v>20.5</v>
       </c>
-      <c r="C89" s="24">
+      <c r="C89" s="23">
         <f t="shared" si="0"/>
-        <v>175.23469478332285</v>
+        <v>198.43333019315301</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="3">
         <v>22</v>
       </c>
-      <c r="C90" s="24">
+      <c r="C90" s="23">
         <f t="shared" si="0"/>
-        <v>206.85678299062511</v>
+        <v>182.94534370872148</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="3">
         <v>23.5</v>
       </c>
-      <c r="C91" s="24">
+      <c r="C91" s="23">
         <f t="shared" si="0"/>
-        <v>162.20765512317175</v>
+        <v>135.02613720319843</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="3">
         <v>25</v>
       </c>
-      <c r="C92" s="24">
+      <c r="C92" s="23">
         <f t="shared" si="0"/>
-        <v>156.63964623617167</v>
+        <v>135.13008342121472</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="3">
         <v>27</v>
       </c>
-      <c r="C93" s="24">
+      <c r="C93" s="23">
         <f t="shared" si="0"/>
-        <v>139.62044926081299</v>
+        <v>130.24461117444773</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="3">
         <v>29</v>
       </c>
-      <c r="C94" s="24">
+      <c r="C94" s="23">
         <f t="shared" si="0"/>
-        <v>181.85327138485121</v>
+        <v>137.31295399955744</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="3">
         <v>31</v>
       </c>
-      <c r="C95" s="24">
+      <c r="C95" s="23">
         <f t="shared" si="0"/>
-        <v>154.22334049275656</v>
+        <v>112.78164654770615</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="3">
         <v>33</v>
       </c>
-      <c r="C96" s="24">
+      <c r="C96" s="23">
         <f t="shared" si="0"/>
-        <v>172.5032187255492</v>
+        <v>139.59977079591647</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B97" s="3">
         <v>35</v>
       </c>
-      <c r="C97" s="24">
+      <c r="C97" s="23">
         <f t="shared" si="0"/>
-        <v>187.21116672894561</v>
+        <v>188.14265460953743</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B98" s="3">
         <v>37</v>
       </c>
-      <c r="C98" s="24">
+      <c r="C98" s="23">
         <f t="shared" si="0"/>
-        <v>139.30527894645448</v>
+        <v>156.64695055059275</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B99" s="3">
         <v>39</v>
       </c>
-      <c r="C99" s="24">
+      <c r="C99" s="23">
         <f t="shared" si="0"/>
-        <v>153.90817017839805</v>
+        <v>130.14066495643144</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B100" s="3">
         <v>41</v>
       </c>
-      <c r="C100" s="24">
+      <c r="C100" s="23">
         <f t="shared" si="0"/>
-        <v>138.56988154628468</v>
+        <v>83.572759285120497</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B101" s="3">
         <v>43</v>
       </c>
-      <c r="C101" s="24">
+      <c r="C101" s="23">
         <f t="shared" si="0"/>
-        <v>136.88897320303937</v>
+        <v>109.45536757118393</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B102" s="3">
         <v>45</v>
       </c>
-      <c r="C102" s="24">
+      <c r="C102" s="23">
         <f t="shared" si="0"/>
-        <v>105.2668849957371</v>
+        <v>109.55931378920026</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2609,7 +2610,7 @@
       </c>
       <c r="C104">
         <f>C73/C$5/($B73-$B72)</f>
-        <v>58739.897502486376</v>
+        <v>69992.574815709551</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2617,8 +2618,8 @@
         <v>2</v>
       </c>
       <c r="C105">
-        <f t="shared" ref="C105:C133" si="1">C74/C$5/($B74-$B73)</f>
-        <v>16710.910901808198</v>
+        <f>C74/C$5/($B74-$B73)</f>
+        <v>18281.452703978935</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2626,8 +2627,8 @@
         <v>3</v>
       </c>
       <c r="C106">
-        <f t="shared" si="1"/>
-        <v>6811.651207010972</v>
+        <f t="shared" ref="C105:C133" si="1">C75/C$5/($B75-$B74)</f>
+        <v>7462.0302868823846</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2636,7 +2637,7 @@
       </c>
       <c r="C107">
         <f t="shared" si="1"/>
-        <v>3484.8894121582921</v>
+        <v>3814.0130165001401</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2645,7 +2646,7 @@
       </c>
       <c r="C108">
         <f t="shared" si="1"/>
-        <v>705.68863455122323</v>
+        <v>2355.2303786248608</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -2654,7 +2655,7 @@
       </c>
       <c r="C109">
         <f t="shared" si="1"/>
-        <v>3073.0905675869781</v>
+        <v>1613.2877306410328</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -2663,7 +2664,7 @@
       </c>
       <c r="C110">
         <f t="shared" si="1"/>
-        <v>1681.3321095646324</v>
+        <v>1093.9101991241189</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2672,7 +2673,7 @@
       </c>
       <c r="C111">
         <f t="shared" si="1"/>
-        <v>1343.1038065436958</v>
+        <v>967.51301225053396</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2681,7 +2682,7 @@
       </c>
       <c r="C112">
         <f t="shared" si="1"/>
-        <v>954.84753526850227</v>
+        <v>867.27915916336917</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
@@ -2690,7 +2691,7 @@
       </c>
       <c r="C113">
         <f t="shared" si="1"/>
-        <v>808.29501650015004</v>
+        <v>608.12073125193433</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
@@ -2699,7 +2700,7 @@
       </c>
       <c r="C114">
         <f t="shared" si="1"/>
-        <v>460.3881000130304</v>
+        <v>461.27607405427733</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
@@ -2708,7 +2709,7 @@
       </c>
       <c r="C115">
         <f t="shared" si="1"/>
-        <v>446.65493225695991</v>
+        <v>295.69281292850837</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
@@ -2717,7 +2718,7 @@
       </c>
       <c r="C116">
         <f t="shared" si="1"/>
-        <v>377.46592518113806</v>
+        <v>339.06266352942151</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
@@ -2726,7 +2727,7 @@
       </c>
       <c r="C117">
         <f t="shared" si="1"/>
-        <v>315.47048216801966</v>
+        <v>317.25988537407119</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
@@ -2735,7 +2736,7 @@
       </c>
       <c r="C118">
         <f t="shared" si="1"/>
-        <v>313.37780898614227</v>
+        <v>257.74419365270938</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
@@ -2744,7 +2745,7 @@
       </c>
       <c r="C119">
         <f t="shared" si="1"/>
-        <v>271.00117705312471</v>
+        <v>224.86324713734317</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
@@ -2753,7 +2754,7 @@
       </c>
       <c r="C120">
         <f t="shared" si="1"/>
-        <v>218.16117921072012</v>
+        <v>224.98109999223695</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
@@ -2762,7 +2763,7 @@
       </c>
       <c r="C121">
         <f t="shared" si="1"/>
-        <v>257.52959344478887</v>
+        <v>207.42102461306288</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
@@ -2771,7 +2772,7 @@
       </c>
       <c r="C122">
         <f t="shared" si="1"/>
-        <v>201.94296205117018</v>
+        <v>153.09085850702766</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
@@ -2780,7 +2781,7 @@
       </c>
       <c r="C123">
         <f t="shared" si="1"/>
-        <v>195.01098213620125</v>
+        <v>153.20871136192144</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
@@ -2789,7 +2790,7 @@
       </c>
       <c r="C124">
         <f t="shared" si="1"/>
-        <v>130.36699962726934</v>
+        <v>110.75222038643513</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
@@ -2798,7 +2799,7 @@
       </c>
       <c r="C125">
         <f t="shared" si="1"/>
-        <v>169.80080989827181</v>
+        <v>116.76271598601821</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
@@ -2807,7 +2808,7 @@
       </c>
       <c r="C126">
         <f t="shared" si="1"/>
-        <v>144.00207332793937</v>
+        <v>95.902760669818136</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
@@ -2816,7 +2817,7 @@
       </c>
       <c r="C127">
         <f t="shared" si="1"/>
-        <v>161.07043896762696</v>
+        <v>118.70728809176569</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
@@ -2825,7 +2826,7 @@
       </c>
       <c r="C128">
         <f t="shared" si="1"/>
-        <v>174.80360672369747</v>
+        <v>159.98525051831413</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -2834,7 +2835,7 @@
       </c>
       <c r="C129">
         <f t="shared" si="1"/>
-        <v>130.07271746106781</v>
+        <v>133.2031892437013</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -2843,7 +2844,7 @@
       </c>
       <c r="C130">
         <f t="shared" si="1"/>
-        <v>143.70779116173784</v>
+        <v>110.66383074526482</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2852,7 +2853,7 @@
       </c>
       <c r="C131">
         <f t="shared" si="1"/>
-        <v>129.38605907326431</v>
+        <v>71.06527150095279</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -2861,7 +2862,7 @@
       </c>
       <c r="C132">
         <f t="shared" si="1"/>
-        <v>127.81655418685625</v>
+        <v>93.074292152367278</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -2870,7 +2871,7 @@
       </c>
       <c r="C133">
         <f t="shared" si="1"/>
-        <v>98.290243511304652</v>
+        <v>93.162681793537629</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -2887,7 +2888,7 @@
       </c>
       <c r="C135">
         <f>LOG10(C104)</f>
-        <v>4.768933184370244</v>
+        <v>4.8450519701913146</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -2896,7 +2897,7 @@
       </c>
       <c r="C136">
         <f t="shared" ref="C136:C164" si="2">LOG10(C105)</f>
-        <v>4.2230001236723682</v>
+        <v>4.2620107032279266</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -2905,7 +2906,7 @@
       </c>
       <c r="C137">
         <f t="shared" si="2"/>
-        <v>3.8332524016586405</v>
+        <v>3.8728570074224731</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -2914,7 +2915,7 @@
       </c>
       <c r="C138">
         <f t="shared" si="2"/>
-        <v>3.5421890009558488</v>
+        <v>3.581382170876882</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -2923,7 +2924,7 @@
       </c>
       <c r="C139">
         <f t="shared" si="2"/>
-        <v>2.8486131229726972</v>
+        <v>3.372033394382973</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -2932,7 +2933,7 @@
       </c>
       <c r="C140">
         <f t="shared" si="2"/>
-        <v>3.4875753596132486</v>
+        <v>3.2077118309262769</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -2941,7 +2942,7 @@
       </c>
       <c r="C141">
         <f t="shared" si="2"/>
-        <v>3.2256535070773844</v>
+        <v>3.0389816715169649</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -2950,7 +2951,7 @@
       </c>
       <c r="C142">
         <f t="shared" si="2"/>
-        <v>3.1281095799560443</v>
+        <v>2.9856568146321401</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -2959,7 +2960,7 @@
       </c>
       <c r="C143">
         <f t="shared" si="2"/>
-        <v>2.9799340313976925</v>
+        <v>2.9381589103600017</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -2968,7 +2969,7 @@
       </c>
       <c r="C144">
         <f t="shared" si="2"/>
-        <v>2.9075699011873208</v>
+        <v>2.7839898090611648</v>
       </c>
     </row>
     <row r="145" spans="2:14" x14ac:dyDescent="0.25">
@@ -2977,7 +2978,7 @@
       </c>
       <c r="C145" s="15">
         <f t="shared" si="2"/>
-        <v>2.6631240895766357</v>
+        <v>2.663960928755936</v>
       </c>
     </row>
     <row r="146" spans="2:14" x14ac:dyDescent="0.25">
@@ -2986,7 +2987,7 @@
       </c>
       <c r="C146">
         <f t="shared" si="2"/>
-        <v>2.6499721341160565</v>
+        <v>2.4708407687485643</v>
       </c>
     </row>
     <row r="147" spans="2:14" x14ac:dyDescent="0.25">
@@ -2995,7 +2996,7 @@
       </c>
       <c r="C147">
         <f t="shared" si="2"/>
-        <v>2.5768777528559803</v>
+        <v>2.5302799693242797</v>
       </c>
     </row>
     <row r="148" spans="2:14" x14ac:dyDescent="0.25">
@@ -3004,7 +3005,7 @@
       </c>
       <c r="C148">
         <f t="shared" si="2"/>
-        <v>2.4989587295666187</v>
+        <v>2.5014151629858929</v>
       </c>
     </row>
     <row r="149" spans="2:14" x14ac:dyDescent="0.25">
@@ -3013,7 +3014,7 @@
       </c>
       <c r="C149">
         <f t="shared" si="2"/>
-        <v>2.4960682398157785</v>
+        <v>2.4111888904715908</v>
       </c>
     </row>
     <row r="150" spans="2:14" x14ac:dyDescent="0.25">
@@ -3022,7 +3023,7 @@
       </c>
       <c r="C150">
         <f t="shared" si="2"/>
-        <v>2.4329711771717002</v>
+        <v>2.3519184778020299</v>
       </c>
     </row>
     <row r="151" spans="2:14" x14ac:dyDescent="0.25">
@@ -3031,7 +3032,7 @@
       </c>
       <c r="C151">
         <f t="shared" si="2"/>
-        <v>2.338777472400225</v>
+        <v>2.3521460358276203</v>
       </c>
     </row>
     <row r="152" spans="2:14" x14ac:dyDescent="0.25">
@@ -3040,7 +3041,7 @@
       </c>
       <c r="C152">
         <f t="shared" si="2"/>
-        <v>2.4108271422366232</v>
+        <v>2.3168527752481034</v>
       </c>
     </row>
     <row r="153" spans="2:14" x14ac:dyDescent="0.25">
@@ -3049,7 +3050,7 @@
       </c>
       <c r="C153">
         <f t="shared" si="2"/>
-        <v>2.3052287220982222</v>
+        <v>2.1849492585069816</v>
       </c>
     </row>
     <row r="154" spans="2:14" x14ac:dyDescent="0.25">
@@ -3058,7 +3059,7 @@
       </c>
       <c r="C154">
         <f t="shared" si="2"/>
-        <v>2.2900590695514995</v>
+        <v>2.1852834597407904</v>
       </c>
     </row>
     <row r="155" spans="2:14" x14ac:dyDescent="0.25">
@@ -3067,7 +3068,7 @@
       </c>
       <c r="C155">
         <f t="shared" si="2"/>
-        <v>2.1151676704329372</v>
+        <v>2.0443524418198038</v>
       </c>
     </row>
     <row r="156" spans="2:14" x14ac:dyDescent="0.25">
@@ -3076,7 +3077,7 @@
       </c>
       <c r="C156">
         <f t="shared" si="2"/>
-        <v>2.229939757365599</v>
+        <v>2.0673041884401808</v>
       </c>
     </row>
     <row r="157" spans="2:14" x14ac:dyDescent="0.25">
@@ -3085,7 +3086,7 @@
       </c>
       <c r="C157">
         <f t="shared" si="2"/>
-        <v>2.1583687450702569</v>
+        <v>1.9818311090102019</v>
       </c>
     </row>
     <row r="158" spans="2:14" x14ac:dyDescent="0.25">
@@ -3094,7 +3095,7 @@
       </c>
       <c r="C158">
         <f t="shared" si="2"/>
-        <v>2.207015842273627</v>
+        <v>2.0744773834943691</v>
       </c>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
@@ -3114,7 +3115,7 @@
       </c>
       <c r="C159">
         <f t="shared" si="2"/>
-        <v>2.2425503891910608</v>
+        <v>2.2040799456948381</v>
       </c>
       <c r="D159" s="11"/>
       <c r="E159" s="11"/>
@@ -3134,7 +3135,7 @@
       </c>
       <c r="C160">
         <f t="shared" si="2"/>
-        <v>2.1141862135589591</v>
+        <v>2.1245146231402856</v>
       </c>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
@@ -3154,7 +3155,7 @@
       </c>
       <c r="C161">
         <f t="shared" si="2"/>
-        <v>2.1574803141803334</v>
+        <v>2.0440056997000644</v>
       </c>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
@@ -3174,7 +3175,7 @@
       </c>
       <c r="C162">
         <f t="shared" si="2"/>
-        <v>2.1118874850365703</v>
+        <v>1.8516574195741049</v>
       </c>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
@@ -3194,7 +3195,7 @@
       </c>
       <c r="C163">
         <f t="shared" si="2"/>
-        <v>2.1065871052027898</v>
+        <v>1.9688297420111402</v>
       </c>
       <c r="D163" s="11"/>
       <c r="E163" s="11"/>
@@ -3214,7 +3215,7 @@
       </c>
       <c r="C164">
         <f t="shared" si="2"/>
-        <v>1.992510411021432</v>
+        <v>1.9692419817021816</v>
       </c>
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
@@ -3253,7 +3254,7 @@
       </c>
       <c r="C166" s="11">
         <f>RSQ($B135:$B$164, $C135:$C$164)</f>
-        <v>0.68507861574197049</v>
+        <v>0.69901701967093721</v>
       </c>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
@@ -3273,7 +3274,7 @@
       </c>
       <c r="C167" s="11">
         <f>RSQ($B136:$B$164, $C136:$C$164)</f>
-        <v>0.72896675230899965</v>
+        <v>0.74524047590941223</v>
       </c>
       <c r="D167" s="11"/>
       <c r="E167" s="11"/>
@@ -3293,7 +3294,7 @@
       </c>
       <c r="C168" s="11">
         <f>RSQ($B137:$B$164, $C137:$C$164)</f>
-        <v>0.75968109449758259</v>
+        <v>0.77778778039499885</v>
       </c>
       <c r="D168" s="12"/>
       <c r="E168" s="12"/>
@@ -3313,7 +3314,7 @@
       </c>
       <c r="C169" s="11">
         <f>RSQ($B138:$B$164, $C138:$C$164)</f>
-        <v>0.77678400574269502</v>
+        <v>0.80090432429986236</v>
       </c>
       <c r="D169" s="11"/>
       <c r="E169" s="11"/>
@@ -3333,7 +3334,7 @@
       </c>
       <c r="C170" s="11">
         <f>RSQ($B139:$B$164, $C139:$C$164)</f>
-        <v>0.78031035089943157</v>
+        <v>0.81505199228096159</v>
       </c>
       <c r="D170" s="11"/>
       <c r="E170" s="11"/>
@@ -3353,7 +3354,7 @@
       </c>
       <c r="C171" s="11">
         <f>RSQ($B140:$B$164, $C140:$C$164)</f>
-        <v>0.77762128461465518</v>
+        <v>0.82338089410775306</v>
       </c>
       <c r="D171" s="11"/>
       <c r="E171" s="11"/>
@@ -3371,9 +3372,9 @@
       <c r="B172" s="3">
         <v>7</v>
       </c>
-      <c r="C172" s="11">
+      <c r="C172" s="13">
         <f>RSQ($B141:$B$164, $C141:$C$164)</f>
-        <v>0.8029521514719643</v>
+        <v>0.82697132814732521</v>
       </c>
       <c r="D172" s="11"/>
       <c r="E172" s="11"/>
@@ -3393,7 +3394,7 @@
       </c>
       <c r="C173" s="11">
         <f>RSQ($B142:$B$164, $C142:$C$164)</f>
-        <v>0.81059461380870124</v>
+        <v>0.82054262337071759</v>
       </c>
       <c r="D173" s="11"/>
       <c r="E173" s="11"/>
@@ -3413,7 +3414,7 @@
       </c>
       <c r="C174" s="11">
         <f>RSQ($B143:$B$164, $C143:$C$164)</f>
-        <v>0.82710738602509837</v>
+        <v>0.81758979681991206</v>
       </c>
       <c r="D174" s="11"/>
       <c r="E174" s="11"/>
@@ -3433,7 +3434,7 @@
       </c>
       <c r="C175" s="11">
         <f>RSQ($B144:$B$164, $C144:$C$164)</f>
-        <v>0.83817290968646141</v>
+        <v>0.82574512000833755</v>
       </c>
       <c r="D175" s="11"/>
       <c r="E175" s="11"/>
@@ -3451,9 +3452,9 @@
       <c r="B176" s="4">
         <v>11.5</v>
       </c>
-      <c r="C176" s="13">
+      <c r="C176" s="33">
         <f>RSQ($B145:$B$164, $C145:$C$164)</f>
-        <v>0.8676488819735938</v>
+        <v>0.81938233122928905</v>
       </c>
       <c r="D176" s="11"/>
       <c r="E176" s="11"/>
@@ -3473,7 +3474,7 @@
       </c>
       <c r="C177" s="11">
         <f>RSQ($B146:$B$164, $C146:$C$164)</f>
-        <v>0.85247779060873785</v>
+        <v>0.80271167391805009</v>
       </c>
       <c r="D177" s="11"/>
       <c r="E177" s="11"/>
@@ -3493,7 +3494,7 @@
       </c>
       <c r="C178" s="11">
         <f>RSQ($B147:$B$164, $C147:$C$164)</f>
-        <v>0.84221306387332007</v>
+        <v>0.77817212836426475</v>
       </c>
       <c r="D178" s="11"/>
       <c r="E178" s="11"/>
@@ -3513,7 +3514,7 @@
       </c>
       <c r="C179" s="11">
         <f>RSQ($B148:$B$164, $C148:$C$164)</f>
-        <v>0.82410007280621367</v>
+        <v>0.74477613806213772</v>
       </c>
       <c r="D179" s="11"/>
       <c r="E179" s="11"/>
@@ -3533,7 +3534,7 @@
       </c>
       <c r="C180" s="11">
         <f>RSQ($B149:$B$164, $C149:$C$164)</f>
-        <v>0.79525681619920119</v>
+        <v>0.70590008718633424</v>
       </c>
       <c r="D180" s="11"/>
       <c r="E180" s="11"/>
@@ -3553,7 +3554,7 @@
       </c>
       <c r="C181" s="11">
         <f>RSQ($B150:$B$164, $C150:$C$164)</f>
-        <v>0.76516381343498885</v>
+        <v>0.65350386863312349</v>
       </c>
       <c r="D181" s="11"/>
       <c r="E181" s="11"/>
@@ -3573,7 +3574,7 @@
       </c>
       <c r="C182" s="11">
         <f>RSQ($B151:$B$164, $C151:$C$164)</f>
-        <v>0.72074082629627134</v>
+        <v>0.59001095303671436</v>
       </c>
       <c r="D182" s="11"/>
       <c r="E182" s="11"/>
@@ -3593,7 +3594,7 @@
       </c>
       <c r="C183" s="11">
         <f>RSQ($B152:$B$164, $C152:$C$164)</f>
-        <v>0.6791920892263702</v>
+        <v>0.50331239906576297</v>
       </c>
       <c r="D183" s="11"/>
       <c r="E183" s="11"/>
@@ -3613,7 +3614,7 @@
       </c>
       <c r="C184" s="11">
         <f>RSQ($B153:$B$164, $C153:$C$164)</f>
-        <v>0.61206827454956181</v>
+        <v>0.38640764624833512</v>
       </c>
       <c r="D184" s="11"/>
       <c r="E184" s="11"/>
@@ -3633,7 +3634,7 @@
       </c>
       <c r="C185" s="11">
         <f>RSQ($B154:$B$164, $C154:$C$164)</f>
-        <v>0.51878738352122888</v>
+        <v>0.29632285052342167</v>
       </c>
       <c r="D185" s="11"/>
       <c r="E185" s="11"/>
@@ -3653,7 +3654,7 @@
       </c>
       <c r="C186" s="11">
         <f>RSQ($B155:$B$164, $C155:$C$164)</f>
-        <v>0.3828399317700486</v>
+        <v>0.17159782717884745</v>
       </c>
       <c r="D186" s="11"/>
       <c r="E186" s="11"/>
@@ -3673,7 +3674,7 @@
       </c>
       <c r="C187" s="11">
         <f>RSQ($B156:$B$164, $C156:$C$164)</f>
-        <v>0.66635606989841367</v>
+        <v>0.21250770461669388</v>
       </c>
     </row>
     <row r="188" spans="2:14" x14ac:dyDescent="0.25">
@@ -3682,7 +3683,7 @@
       </c>
       <c r="C188" s="11">
         <f>RSQ($B157:$B$164, $C157:$C$164)</f>
-        <v>0.60429264522578774</v>
+        <v>0.2208978245985227</v>
       </c>
     </row>
     <row r="189" spans="2:14" x14ac:dyDescent="0.25">
@@ -3691,7 +3692,7 @@
       </c>
       <c r="C189" s="11">
         <f>RSQ($B158:$B$164, $C158:$C$164)</f>
-        <v>0.76514286370293227</v>
+        <v>0.49731493168021551</v>
       </c>
     </row>
     <row r="190" spans="2:14" x14ac:dyDescent="0.25">
@@ -3700,7 +3701,7 @@
       </c>
       <c r="C190" s="11">
         <f>RSQ($B159:$B$164, $C159:$C$164)</f>
-        <v>0.75377214398859171</v>
+        <v>0.61090351594599912</v>
       </c>
     </row>
     <row r="191" spans="2:14" x14ac:dyDescent="0.25">
@@ -3709,7 +3710,7 @@
       </c>
       <c r="C191" s="11">
         <f>RSQ($B160:$B$164, $C160:$C$164)</f>
-        <v>0.57021473943163126</v>
+        <v>0.36274806044285957</v>
       </c>
       <c r="D191" s="11"/>
       <c r="E191" s="11"/>
@@ -3729,7 +3730,7 @@
       </c>
       <c r="C192" s="11">
         <f>RSQ($B161:$B$164, $C161:$C$164)</f>
-        <v>0.84564210865157929</v>
+        <v>3.0277754455740401E-2</v>
       </c>
       <c r="D192" s="11"/>
       <c r="E192" s="11"/>
@@ -3749,7 +3750,7 @@
       </c>
       <c r="C193" s="11">
         <f>RSQ($B162:$B$164, $C162:$C$164)</f>
-        <v>0.78323168068499527</v>
+        <v>0.75262939240603344</v>
       </c>
       <c r="D193" s="11"/>
       <c r="E193" s="11"/>
@@ -3804,7 +3805,7 @@
         <v>16</v>
       </c>
       <c r="C196">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D196" s="11"/>
       <c r="E196" s="11"/>
@@ -3857,7 +3858,7 @@
       </c>
       <c r="C200" s="11">
         <f>RSQ($B$135:$B137, $C$135:$C137)</f>
-        <v>0.99079785839474788</v>
+        <v>0.98691565488333755</v>
       </c>
     </row>
     <row r="201" spans="1:14" x14ac:dyDescent="0.25">
@@ -3866,44 +3867,32 @@
       </c>
       <c r="C201" s="11">
         <f>RSQ($B$135:$B138, $C$135:$C138)</f>
-        <v>0.98057762258840753</v>
+        <v>0.97574775376255696</v>
       </c>
     </row>
     <row r="202" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B202" s="3">
         <v>5</v>
       </c>
-      <c r="C202" s="11">
-        <f>RSQ($B$135:$B139, $C$135:$C139)</f>
-        <v>0.98232335949957461</v>
-      </c>
+      <c r="C202" s="11"/>
     </row>
     <row r="203" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B203" s="3">
         <v>6</v>
       </c>
-      <c r="C203" s="11">
-        <f>RSQ($B$135:$B140, $C$135:$C140)</f>
-        <v>0.76503728239003888</v>
-      </c>
+      <c r="C203" s="11"/>
     </row>
     <row r="204" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B204" s="3">
         <v>7</v>
       </c>
-      <c r="C204" s="11">
-        <f>RSQ($B$135:$B141, $C$135:$C141)</f>
-        <v>0.7307098410640902</v>
-      </c>
+      <c r="C204" s="12"/>
     </row>
     <row r="205" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B205" s="3">
         <v>8</v>
       </c>
-      <c r="C205" s="11">
-        <f>RSQ($B$135:$B142, $C$135:$C142)</f>
-        <v>0.71877135816859516</v>
-      </c>
+      <c r="C205" s="11"/>
     </row>
     <row r="206" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B206" s="3">
@@ -4041,18 +4030,18 @@
       <c r="B231" s="3">
         <v>3</v>
       </c>
-      <c r="C231">
-        <f>RSQ($B137:$B$144, C137:C$144)</f>
-        <v>0.53276243958482195</v>
+      <c r="C231" s="23">
+        <f>RSQ($B137:$B$140, C137:C$140)</f>
+        <v>0.98336814149626794</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B232" s="4">
         <v>4</v>
       </c>
-      <c r="C232">
-        <f>RSQ($B138:$B$144, C138:C$144)</f>
-        <v>0.31640544623194478</v>
+      <c r="C232" s="23">
+        <f>RSQ($B138:$B$140, C138:C$140)</f>
+        <v>0.9951832436320065</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -4060,44 +4049,28 @@
         <v>5</v>
       </c>
       <c r="C233">
-        <f>RSQ($B139:$B$144, C139:C$144)</f>
-        <v>8.9235146548653069E-2</v>
+        <f>RSQ($B139:$B$140, C139:C$140)</f>
+        <v>0.99999999999999956</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B234" s="3">
         <v>6</v>
       </c>
-      <c r="C234">
-        <f>RSQ($B140:$B$144, C140:C$144)</f>
-        <v>0.95111193080715106</v>
-      </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B235" s="3">
         <v>7</v>
       </c>
-      <c r="C235">
-        <f>RSQ($B141:$B$144, C141:C$144)</f>
-        <v>0.98448122760404067</v>
-      </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B236" s="3">
         <v>8</v>
       </c>
-      <c r="C236">
-        <f>RSQ($B142:$B$144, C142:C$144)</f>
-        <v>0.96210373452020703</v>
-      </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B237" s="3">
         <v>9</v>
-      </c>
-      <c r="C237">
-        <f>RSQ($B143:$B$144, C143:C$144)</f>
-        <v>0.99999999999999956</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -4307,7 +4280,7 @@
       </c>
       <c r="C262" s="11">
         <f>SUM(C199,C231)</f>
-        <v>1.5327624395848218</v>
+        <v>1.9833681414962681</v>
       </c>
     </row>
     <row r="263" spans="1:14" x14ac:dyDescent="0.25">
@@ -4315,54 +4288,42 @@
         <v>4</v>
       </c>
       <c r="C263" s="11">
-        <f t="shared" ref="C263:C268" si="3">SUM(C200,C232)</f>
-        <v>1.3072033046266927</v>
+        <f t="shared" ref="C263:C264" si="3">SUM(C200,C232)</f>
+        <v>1.982098898515344</v>
       </c>
     </row>
     <row r="264" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B264" s="3">
         <v>5</v>
       </c>
-      <c r="C264" s="16">
+      <c r="C264" s="11">
         <f>SUM(C201,C233)</f>
-        <v>1.0698127691370607</v>
+        <v>1.9757477537625565</v>
       </c>
     </row>
     <row r="265" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B265" s="3">
         <v>6</v>
       </c>
-      <c r="C265" s="11">
-        <f>SUM(C202,C234)</f>
-        <v>1.9334352903067256</v>
-      </c>
+      <c r="C265" s="11"/>
     </row>
     <row r="266" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B266" s="3">
         <v>7</v>
       </c>
-      <c r="C266" s="11">
-        <f t="shared" si="3"/>
-        <v>1.7495185099940795</v>
-      </c>
+      <c r="C266" s="11"/>
     </row>
     <row r="267" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B267" s="3">
         <v>8</v>
       </c>
-      <c r="C267" s="11">
-        <f t="shared" si="3"/>
-        <v>1.6928135755842972</v>
-      </c>
+      <c r="C267" s="11"/>
     </row>
     <row r="268" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B268" s="3">
         <v>9</v>
       </c>
-      <c r="C268" s="11">
-        <f t="shared" si="3"/>
-        <v>1.7187713581685946</v>
-      </c>
+      <c r="C268" s="11"/>
     </row>
     <row r="269" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B269" s="4">
@@ -4475,7 +4436,7 @@
       </c>
       <c r="C290">
         <f>MAX(C259:C289)</f>
-        <v>1.9334352903067256</v>
+        <v>1.9833681414962681</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -4484,7 +4445,7 @@
       </c>
       <c r="C291">
         <f>MATCH(C290,C260:C268,0)-1</f>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -4501,7 +4462,7 @@
       </c>
       <c r="C293">
         <f t="shared" ref="C293:C298" si="4">IF(0 &lt; 10^C135-10^(C$19*$B293+C$20), LOG(10^C135-10^(C$19*$B293+C$20)), 0)</f>
-        <v>4.7646509629405287</v>
+        <v>4.8395986359347383</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -4510,7 +4471,7 @@
       </c>
       <c r="C294">
         <f t="shared" si="4"/>
-        <v>4.2083677949473088</v>
+        <v>4.242030064343707</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -4519,7 +4480,7 @@
       </c>
       <c r="C295">
         <f t="shared" si="4"/>
-        <v>3.7979459407249321</v>
+        <v>3.8253189921428397</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -4528,7 +4489,7 @@
       </c>
       <c r="C296">
         <f t="shared" si="4"/>
-        <v>3.4733380903149476</v>
+        <v>3.4893722889253067</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -4537,7 +4498,7 @@
       </c>
       <c r="C297">
         <f t="shared" si="4"/>
-        <v>2.3322269814558161</v>
+        <v>3.2226834440092555</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -4546,7 +4507,7 @@
       </c>
       <c r="C298">
         <f t="shared" si="4"/>
-        <v>3.4152440369300603</v>
+        <v>2.9859810086009557</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -4555,7 +4516,7 @@
       </c>
       <c r="C299">
         <f>IF(0 &lt; 10^C141-10^(C$19*$B299+C$20), LOG(10^C141-10^(C$19*$B299+C$20)), 0)</f>
-        <v>3.0893488371182234</v>
+        <v>2.6873441790479209</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -4564,7 +4525,7 @@
       </c>
       <c r="C300">
         <f t="shared" ref="C300:C302" si="5">IF(0 &lt; 10^C142-10^(C$19*$B300+C$20), LOG(10^C142-10^(C$19*$B300+C$20)), 0)</f>
-        <v>2.9580998716769247</v>
+        <v>2.5978043972355183</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -4573,7 +4534,7 @@
       </c>
       <c r="C301">
         <f t="shared" si="5"/>
-        <v>2.7298958599953789</v>
+        <v>2.5178158400620561</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -4582,7 +4543,7 @@
       </c>
       <c r="C302">
         <f t="shared" si="5"/>
-        <v>2.6093874080003832</v>
+        <v>2.0083426980731613</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -4687,7 +4648,7 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B323" s="3">
         <v>0</v>
@@ -4698,8 +4659,8 @@
         <v>1</v>
       </c>
       <c r="C324">
-        <f t="shared" ref="C324:C326" si="6">IF(0&lt;10^C293-10^(C$28*$B324+C$29),LOG(10^C293-10^(C$28*$B324+C$29)),0)</f>
-        <v>4.5596107866378981</v>
+        <f t="shared" ref="C324:C325" si="6">IF(0&lt;10^C293-10^(C$28*$B324+C$29),LOG(10^C293-10^(C$28*$B324+C$29)),0)</f>
+        <v>4.6669618407554641</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -4708,7 +4669,7 @@
       </c>
       <c r="C325">
         <f t="shared" si="6"/>
-        <v>3.3530883260033879</v>
+        <v>3.7418719455152729</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>